<commit_message>
Fixed Bug on Emissions and Duplicated Damage
</commit_message>
<xml_diff>
--- a/CreateDB_NC/InputData/FragilityCurvesData/Tech2FragilityCurve.xlsx
+++ b/CreateDB_NC/InputData/FragilityCurvesData/Tech2FragilityCurve.xlsx
@@ -1,24 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor\Desktop\TEMOA\TemoaHurricane_V2\CreateDB_NC\InputData\FragilityCurvesData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Remote\Desktop\Projects\TemoaHurricane_OEA\TEMOA_GIT\TemoaHurricane_V2\CreateDB_NC\InputData\FragilityCurvesData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C53ED2C-3C8B-4D3C-9065-FE6F73894983}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7921C128-BF2D-4DA0-A6D2-1D7FC034A55D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -721,18 +732,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{403AAC54-22D7-42C6-84BF-5B756562A678}">
   <dimension ref="A1:C56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.3984375" customWidth="1"/>
+    <col min="1" max="1" width="36.42578125" customWidth="1"/>
     <col min="2" max="2" width="47" customWidth="1"/>
-    <col min="3" max="3" width="21.3984375" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -743,7 +754,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -754,604 +765,601 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" t="s">
+        <v>91</v>
+      </c>
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" t="s">
+        <v>92</v>
+      </c>
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" t="s">
+        <v>97</v>
+      </c>
+      <c r="C13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" t="s">
+        <v>101</v>
+      </c>
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" t="s">
+        <v>102</v>
+      </c>
+      <c r="C15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" t="s">
+        <v>105</v>
+      </c>
+      <c r="C16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" t="s">
+        <v>109</v>
+      </c>
+      <c r="C17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" t="s">
+        <v>112</v>
+      </c>
+      <c r="C18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" t="s">
+        <v>114</v>
+      </c>
+      <c r="C19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" t="s">
+        <v>116</v>
+      </c>
+      <c r="C20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" t="s">
+        <v>117</v>
+      </c>
+      <c r="C21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>66</v>
+      </c>
+      <c r="B22" t="s">
+        <v>120</v>
+      </c>
+      <c r="C22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>15</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B23" t="s">
         <v>68</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C23" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>16</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B24" t="s">
         <v>69</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C24" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>17</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B25" t="s">
         <v>70</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C25" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>18</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B26" t="s">
         <v>71</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C26" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>19</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B27" t="s">
         <v>72</v>
       </c>
-      <c r="C7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
+      <c r="C27" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>20</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B28" t="s">
         <v>73</v>
       </c>
-      <c r="C8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" t="s">
-        <v>74</v>
-      </c>
-      <c r="C9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" t="s">
-        <v>75</v>
-      </c>
-      <c r="C10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
+      <c r="C28" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>23</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B29" t="s">
         <v>5</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C29" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>24</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B30" t="s">
         <v>76</v>
       </c>
-      <c r="C12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
+      <c r="C30" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>25</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B31" t="s">
         <v>77</v>
       </c>
-      <c r="C13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
+      <c r="C31" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>26</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B32" t="s">
         <v>78</v>
       </c>
-      <c r="C14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" t="s">
-        <v>79</v>
-      </c>
-      <c r="C15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" t="s">
-        <v>80</v>
-      </c>
-      <c r="C16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
+      <c r="C32" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>31</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B33" t="s">
         <v>82</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C33" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>3</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B34" t="s">
         <v>83</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C34" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A20" t="s">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>32</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B35" t="s">
         <v>84</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C35" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A21" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>4</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B36" t="s">
         <v>85</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C36" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A22" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>33</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B37" t="s">
         <v>86</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C37" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A23" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>34</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B38" t="s">
         <v>87</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C38" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A24" t="s">
-        <v>36</v>
-      </c>
-      <c r="B24" t="s">
-        <v>88</v>
-      </c>
-      <c r="C24" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A25" t="s">
-        <v>37</v>
-      </c>
-      <c r="B25" t="s">
-        <v>89</v>
-      </c>
-      <c r="C25" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A26" t="s">
-        <v>38</v>
-      </c>
-      <c r="B26" t="s">
-        <v>90</v>
-      </c>
-      <c r="C26" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A27" t="s">
-        <v>39</v>
-      </c>
-      <c r="B27" t="s">
-        <v>91</v>
-      </c>
-      <c r="C27" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A28" t="s">
-        <v>40</v>
-      </c>
-      <c r="B28" t="s">
-        <v>92</v>
-      </c>
-      <c r="C28" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A29" t="s">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>41</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B39" t="s">
         <v>93</v>
       </c>
-      <c r="C29" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A30" t="s">
+      <c r="C39" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>42</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B40" t="s">
         <v>94</v>
       </c>
-      <c r="C30" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A31" t="s">
+      <c r="C40" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>43</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B41" t="s">
         <v>95</v>
       </c>
-      <c r="C31" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A32" t="s">
+      <c r="C41" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>44</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B42" t="s">
         <v>96</v>
       </c>
-      <c r="C32" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A33" t="s">
-        <v>45</v>
-      </c>
-      <c r="B33" t="s">
-        <v>97</v>
-      </c>
-      <c r="C33" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A34" t="s">
+      <c r="C42" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>46</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B43" t="s">
         <v>98</v>
       </c>
-      <c r="C34" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A35" t="s">
+      <c r="C43" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>47</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B44" t="s">
         <v>99</v>
       </c>
-      <c r="C35" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A36" t="s">
+      <c r="C44" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>48</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B45" t="s">
         <v>100</v>
       </c>
-      <c r="C36" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A37" t="s">
-        <v>49</v>
-      </c>
-      <c r="B37" t="s">
-        <v>101</v>
-      </c>
-      <c r="C37" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A38" t="s">
-        <v>50</v>
-      </c>
-      <c r="B38" t="s">
-        <v>102</v>
-      </c>
-      <c r="C38" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A39" t="s">
+      <c r="C45" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>51</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B46" t="s">
         <v>103</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C46" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A40" t="s">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>52</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B47" t="s">
         <v>104</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C47" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A41" t="s">
-        <v>53</v>
-      </c>
-      <c r="B41" t="s">
-        <v>105</v>
-      </c>
-      <c r="C41" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A42" t="s">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>27</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B48" t="s">
         <v>106</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C48" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A43" t="s">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>55</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B49" t="s">
         <v>107</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C49" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A44" t="s">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>59</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B50" t="s">
         <v>108</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C50" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A45" t="s">
-        <v>56</v>
-      </c>
-      <c r="B45" t="s">
-        <v>109</v>
-      </c>
-      <c r="C45" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A46" t="s">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>57</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B51" t="s">
         <v>110</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C51" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A47" t="s">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>58</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B52" t="s">
         <v>111</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C52" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A48" t="s">
-        <v>60</v>
-      </c>
-      <c r="B48" t="s">
-        <v>112</v>
-      </c>
-      <c r="C48" t="s">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>61</v>
+      </c>
+      <c r="B53" t="s">
+        <v>113</v>
+      </c>
+      <c r="C53" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A49" t="s">
-        <v>61</v>
-      </c>
-      <c r="B49" t="s">
-        <v>113</v>
-      </c>
-      <c r="C49" t="s">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>63</v>
+      </c>
+      <c r="B54" t="s">
+        <v>115</v>
+      </c>
+      <c r="C54" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A50" t="s">
-        <v>62</v>
-      </c>
-      <c r="B50" t="s">
-        <v>114</v>
-      </c>
-      <c r="C50" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A51" t="s">
-        <v>63</v>
-      </c>
-      <c r="B51" t="s">
-        <v>115</v>
-      </c>
-      <c r="C51" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A52" t="s">
-        <v>64</v>
-      </c>
-      <c r="B52" t="s">
-        <v>116</v>
-      </c>
-      <c r="C52" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A53" t="s">
-        <v>65</v>
-      </c>
-      <c r="B53" t="s">
-        <v>117</v>
-      </c>
-      <c r="C53" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A54" t="s">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>35</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B55" t="s">
         <v>118</v>
-      </c>
-      <c r="C54" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A55" t="s">
-        <v>54</v>
-      </c>
-      <c r="B55" t="s">
-        <v>119</v>
       </c>
       <c r="C55" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C56" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C56">
-    <sortCondition ref="A2:A56"/>
-  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updates on Distribution/Transmission Costs
</commit_message>
<xml_diff>
--- a/CreateDB_NC/InputData/FragilityCurvesData/Tech2FragilityCurve.xlsx
+++ b/CreateDB_NC/InputData/FragilityCurvesData/Tech2FragilityCurve.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Remote\Desktop\Projects\TemoaHurricane_OEA\TEMOA_GIT\TemoaHurricane_V2\CreateDB_NC\InputData\FragilityCurvesData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D36E93F6-9F2E-48E9-85C8-4105A7A843D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D48EF142-4A23-40B9-8F8A-B18133D573E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11400" yWindow="3990" windowWidth="27000" windowHeight="17010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="140">
   <si>
     <t>Technologies</t>
   </si>
@@ -383,9 +383,6 @@
     <t>solar_Kabre</t>
   </si>
   <si>
-    <t>wind_AVG_CAMPO_MIGUEL</t>
-  </si>
-  <si>
     <t>NotAffected</t>
   </si>
   <si>
@@ -447,6 +444,18 @@
   </si>
   <si>
     <t>BIT_ST_EX_RFIT</t>
+  </si>
+  <si>
+    <t>wind_land_Bouchard</t>
+  </si>
+  <si>
+    <t>wind_offshore_Massachusetts_Wilkie</t>
+  </si>
+  <si>
+    <t>Transmission60_Substation40</t>
+  </si>
+  <si>
+    <t>DistributionPole_Wood_Salmana_20Underground</t>
   </si>
 </sst>
 </file>
@@ -737,7 +746,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="39">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -921,12 +930,6 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
@@ -1287,7 +1290,7 @@
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="35" borderId="10"/>
+    <xf numFmtId="0" fontId="2" fillId="34" borderId="10"/>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1458,7 +1461,7 @@
     <xf numFmtId="9" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1467,12 +1470,11 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2129,8 +2131,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{403AAC54-22D7-42C6-84BF-5B756562A678}">
   <dimension ref="A1:C72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59:A72"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2379,7 +2381,7 @@
         <v>109</v>
       </c>
       <c r="C22" t="s">
-        <v>115</v>
+        <v>136</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -2456,7 +2458,7 @@
         <v>5</v>
       </c>
       <c r="C29" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -2500,7 +2502,7 @@
         <v>72</v>
       </c>
       <c r="C33" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -2511,7 +2513,7 @@
         <v>73</v>
       </c>
       <c r="C34" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -2522,7 +2524,7 @@
         <v>74</v>
       </c>
       <c r="C35" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -2533,7 +2535,7 @@
         <v>75</v>
       </c>
       <c r="C36" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -2544,7 +2546,7 @@
         <v>76</v>
       </c>
       <c r="C37" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -2648,7 +2650,7 @@
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B47" t="s">
         <v>95</v>
@@ -2659,7 +2661,7 @@
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B48" t="s">
         <v>96</v>
@@ -2709,7 +2711,7 @@
         <v>107</v>
       </c>
       <c r="C52" t="s">
-        <v>115</v>
+        <v>136</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -2720,7 +2722,7 @@
         <v>108</v>
       </c>
       <c r="C53" t="s">
-        <v>115</v>
+        <v>137</v>
       </c>
     </row>
     <row r="54" spans="1:3" s="3" customFormat="1">
@@ -2731,170 +2733,170 @@
         <v>71</v>
       </c>
       <c r="C54" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" t="s">
+        <v>47</v>
+      </c>
+      <c r="B55" t="s">
+        <v>99</v>
+      </c>
+      <c r="C55" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" t="s">
+        <v>48</v>
+      </c>
+      <c r="B56" t="s">
+        <v>100</v>
+      </c>
+      <c r="C56" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" s="3" customFormat="1">
-      <c r="A55" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C55" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" s="3" customFormat="1">
-      <c r="A56" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="C56" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3">
-      <c r="A57" s="4" t="s">
+      <c r="B57" t="s">
+        <v>118</v>
+      </c>
+      <c r="C57" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" t="s">
         <v>117</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B58" t="s">
         <v>119</v>
       </c>
-      <c r="C57" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3">
-      <c r="A58" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="B58" s="4" t="s">
-        <v>120</v>
-      </c>
       <c r="C58" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="59" spans="1:3">
-      <c r="A59" s="6" t="s">
+      <c r="A59" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B59" s="4"/>
+      <c r="C59" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="B59" s="5"/>
-      <c r="C59" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3">
-      <c r="A60" s="6" t="s">
+      <c r="B60" s="4"/>
+      <c r="C60" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B61" s="4"/>
+      <c r="C61" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B62" s="4"/>
+      <c r="C62" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B63" s="4"/>
+      <c r="C63" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="B60" s="5"/>
-      <c r="C60" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3">
-      <c r="A61" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="B61" s="5"/>
-      <c r="C61" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3">
-      <c r="A62" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="B62" s="5"/>
-      <c r="C62" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3">
-      <c r="A63" s="6" t="s">
+      <c r="B64" s="4"/>
+      <c r="C64" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="B63" s="5"/>
-      <c r="C63" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3">
-      <c r="A64" s="6" t="s">
+      <c r="B65" s="4"/>
+      <c r="C65" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="B64" s="5"/>
-      <c r="C64" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3">
-      <c r="A65" s="6" t="s">
+      <c r="B66" s="4"/>
+      <c r="C66" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B67" s="4"/>
+      <c r="C67" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="B65" s="5"/>
-      <c r="C65" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3">
-      <c r="A66" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="B66" s="5"/>
-      <c r="C66" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3">
-      <c r="A67" s="7" t="s">
+      <c r="B68" s="4"/>
+      <c r="C68" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="C69" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="C70" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="B67" s="5"/>
-      <c r="C67" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3">
-      <c r="A68" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="B68" s="5"/>
-      <c r="C68" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3">
-      <c r="A69" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="C69" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3">
-      <c r="A70" s="7" t="s">
+      <c r="C71" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" s="6" t="s">
         <v>129</v>
-      </c>
-      <c r="C70" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3">
-      <c r="A71" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="C71" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3">
-      <c r="A72" s="7" t="s">
-        <v>130</v>
       </c>
       <c r="C72" t="s">
         <v>110</v>

</xml_diff>

<commit_message>
Small Update Fragility Table
</commit_message>
<xml_diff>
--- a/CreateDB_NC/InputData/FragilityCurvesData/Tech2FragilityCurve.xlsx
+++ b/CreateDB_NC/InputData/FragilityCurvesData/Tech2FragilityCurve.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Remote\Desktop\Projects\TemoaHurricane_OEA\TEMOA_GIT\TemoaHurricane_V2\CreateDB_NC\InputData\FragilityCurvesData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D48EF142-4A23-40B9-8F8A-B18133D573E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{283F59EC-926E-4F68-A1CF-FED1F7AB4B9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11400" yWindow="3990" windowWidth="27000" windowHeight="17010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="142">
   <si>
     <t>Technologies</t>
   </si>
@@ -389,15 +389,9 @@
     <t>GENERAL_CO2_CAP</t>
   </si>
   <si>
-    <t>ENERGY_INTERCHANGE</t>
-  </si>
-  <si>
     <t>Tech Used to Represent Other Options For CO2 Capture</t>
   </si>
   <si>
-    <t>Interchange of Energy in/out of NC</t>
-  </si>
-  <si>
     <t>PV-RESIDENTIAL</t>
   </si>
   <si>
@@ -456,6 +450,18 @@
   </si>
   <si>
     <t>DistributionPole_Wood_Salmana_20Underground</t>
+  </si>
+  <si>
+    <t>ENERGY_IMPORT_S1</t>
+  </si>
+  <si>
+    <t>ENERGY_IMPORT_S2</t>
+  </si>
+  <si>
+    <t>Electricity import to NC - S1 Tracks capacity</t>
+  </si>
+  <si>
+    <t>Electricity import to NC - S2 Tracks emissions. Which vary with the period not the vintage</t>
   </si>
 </sst>
 </file>
@@ -468,7 +474,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="39">
+  <fonts count="40">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -744,6 +750,13 @@
       <color rgb="FF7F7F7F"/>
       <name val="Helvetica Neue"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="38">
@@ -1461,7 +1474,7 @@
     <xf numFmtId="9" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1477,6 +1490,7 @@
     <xf numFmtId="0" fontId="18" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="345">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2129,10 +2143,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{403AAC54-22D7-42C6-84BF-5B756562A678}">
-  <dimension ref="A1:C72"/>
+  <dimension ref="A1:C73"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+      <selection activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2381,7 +2395,7 @@
         <v>109</v>
       </c>
       <c r="C22" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -2650,7 +2664,7 @@
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B47" t="s">
         <v>95</v>
@@ -2661,7 +2675,7 @@
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B48" t="s">
         <v>96</v>
@@ -2711,7 +2725,7 @@
         <v>107</v>
       </c>
       <c r="C52" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -2722,7 +2736,7 @@
         <v>108</v>
       </c>
       <c r="C53" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="54" spans="1:3" s="3" customFormat="1">
@@ -2733,7 +2747,7 @@
         <v>71</v>
       </c>
       <c r="C54" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -2744,7 +2758,7 @@
         <v>99</v>
       </c>
       <c r="C55" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -2755,7 +2769,7 @@
         <v>100</v>
       </c>
       <c r="C56" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -2763,35 +2777,37 @@
         <v>116</v>
       </c>
       <c r="B57" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C57" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="58" spans="1:3">
-      <c r="A58" t="s">
-        <v>117</v>
+      <c r="A58" s="7" t="s">
+        <v>138</v>
       </c>
       <c r="B58" t="s">
-        <v>119</v>
+        <v>140</v>
       </c>
       <c r="C58" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="59" spans="1:3">
-      <c r="A59" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="B59" s="4"/>
+      <c r="A59" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="B59" t="s">
+        <v>141</v>
+      </c>
       <c r="C59" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" s="5" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B60" s="4"/>
       <c r="C60" t="s">
@@ -2800,7 +2816,7 @@
     </row>
     <row r="61" spans="1:3">
       <c r="A61" s="5" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="B61" s="4"/>
       <c r="C61" t="s">
@@ -2809,7 +2825,7 @@
     </row>
     <row r="62" spans="1:3">
       <c r="A62" s="5" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B62" s="4"/>
       <c r="C62" t="s">
@@ -2818,7 +2834,7 @@
     </row>
     <row r="63" spans="1:3">
       <c r="A63" s="5" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B63" s="4"/>
       <c r="C63" t="s">
@@ -2827,7 +2843,7 @@
     </row>
     <row r="64" spans="1:3">
       <c r="A64" s="5" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="B64" s="4"/>
       <c r="C64" t="s">
@@ -2836,7 +2852,7 @@
     </row>
     <row r="65" spans="1:3">
       <c r="A65" s="5" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B65" s="4"/>
       <c r="C65" t="s">
@@ -2844,17 +2860,17 @@
       </c>
     </row>
     <row r="66" spans="1:3">
-      <c r="A66" s="6" t="s">
-        <v>133</v>
+      <c r="A66" s="5" t="s">
+        <v>123</v>
       </c>
       <c r="B66" s="4"/>
       <c r="C66" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" s="6" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B67" s="4"/>
       <c r="C67" t="s">
@@ -2863,7 +2879,7 @@
     </row>
     <row r="68" spans="1:3">
       <c r="A68" s="6" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="B68" s="4"/>
       <c r="C68" t="s">
@@ -2872,15 +2888,16 @@
     </row>
     <row r="69" spans="1:3">
       <c r="A69" s="6" t="s">
-        <v>127</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="B69" s="4"/>
       <c r="C69" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" s="6" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C70" t="s">
         <v>110</v>
@@ -2888,7 +2905,7 @@
     </row>
     <row r="71" spans="1:3">
       <c r="A71" s="6" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="C71" t="s">
         <v>110</v>
@@ -2896,9 +2913,17 @@
     </row>
     <row r="72" spans="1:3">
       <c r="A72" s="6" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="C72" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="C73" t="s">
         <v>110</v>
       </c>
     </row>

</xml_diff>